<commit_message>
updated graphs an excel readout
</commit_message>
<xml_diff>
--- a/Graph Data Visualised.xlsx
+++ b/Graph Data Visualised.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahgonsenhauser/Dropbox/UCT/CSC2001F/Assignment5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4DCC20-FCAD-2645-963F-CDF7A85EB05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E5460C-6E00-504B-91EB-E2960E93B896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{D305D5BE-1447-6B45-9963-199F3DD44BDD}"/>
   </bookViews>
@@ -40,8 +40,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{BF15FC33-5ACD-3F47-A51F-40527AEB8A27}" name="Djikstraout" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr sourceFile="/Users/noahgonsenhauser/Dropbox/UCT/CSC2001F/Assignment5/Djikstraout.txt" decimal="," thousands=" " tab="0" space="1" consecutive="1">
+  <connection id="1" xr16:uid="{38526DA4-F952-E341-9F1B-A50F21DB8BBC}" name="Djikstraout" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/noahgonsenhauser/Dropbox/UCT/CSC2001F/Assignment5/Djikstraout.txt" decimal="," thousands=" " tab="0" space="1" consecutive="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -637,10 +637,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10</c:v>
@@ -829,10 +829,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>38</c:v>
@@ -1021,154 +1021,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>52</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>53</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>87</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>99</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>121</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>119</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>114</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>117</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>148</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>126</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>159</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>219</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>225</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>214</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>279</c:v>
+                  <c:v>293</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>249</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>243</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>245</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>272</c:v>
+                  <c:v>239</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>262</c:v>
+                  <c:v>232</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>292</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>281</c:v>
+                  <c:v>381</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>318</c:v>
+                  <c:v>342</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>380</c:v>
+                  <c:v>332</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>395</c:v>
+                  <c:v>379</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>371</c:v>
+                  <c:v>379</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>384</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>454</c:v>
+                  <c:v>424</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>355</c:v>
+                  <c:v>439</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>421</c:v>
+                  <c:v>385</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>431</c:v>
+                  <c:v>439</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>412</c:v>
+                  <c:v>407</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>441</c:v>
+                  <c:v>532</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>530</c:v>
+                  <c:v>508</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>561</c:v>
+                  <c:v>575</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>542</c:v>
+                  <c:v>575</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>611</c:v>
+                  <c:v>486</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>545</c:v>
+                  <c:v>587</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>600</c:v>
+                  <c:v>575</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>556</c:v>
+                  <c:v>549</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>580</c:v>
+                  <c:v>608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1945,154 +1945,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>33</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>27</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>62</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>72</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>79</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>84</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>77</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>72</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>109</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>86</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>96</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>142</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>154</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>163</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>181</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>151</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>174</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>163</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>164</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>186</c:v>
-                </c:pt>
                 <c:pt idx="30">
-                  <c:v>222</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>243</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>237</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>250</c:v>
+                  <c:v>252</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>236</c:v>
+                  <c:v>252</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>221</c:v>
+                  <c:v>259</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>249</c:v>
+                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>229</c:v>
+                  <c:v>311</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>233</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>242</c:v>
+                  <c:v>253</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>276</c:v>
+                  <c:v>313</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>310</c:v>
+                  <c:v>361</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>351</c:v>
+                  <c:v>376</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>370</c:v>
+                  <c:v>382</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>337</c:v>
+                  <c:v>378</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>326</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>315</c:v>
+                  <c:v>343</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>350</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>333</c:v>
+                  <c:v>298</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>337</c:v>
+                  <c:v>332</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2291,6 +2291,641 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PQOperations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>342</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>391</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>508</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>587</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>549</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>608</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4B16-8B4F-B8CB-8FB0C68535EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>O Complexity (|E|log|V|)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>135.30711954905405</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>166.5318394449896</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>197.75655934092515</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>228.9812792368607</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>260.20599913279625</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>291.4307190287318</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>322.65543892466735</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>353.8801588206029</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>385.10487871653845</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>416.329598612474</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>345.64637360440099</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>425.41092135926277</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>505.17546911412455</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>584.94001686898628</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>664.70456462384811</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>744.46911237870984</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>824.23366013357156</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>903.9982078884334</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>983.76275564329512</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1063.5273033981568</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>666.45695639243229</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>820.25471555991669</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>974.05247472740109</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1127.8502338948854</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1281.6479930623698</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1435.4457522298542</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1589.2435113973386</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1743.041270564823</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1896.8390297323074</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2050.6367888997916</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1104.3305028184122</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1359.176003468815</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1614.0215041192178</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1868.8670047696205</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2123.7125054200233</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2378.558006070426</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2633.4035067208292</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2888.249007371232</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3143.0945080216347</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3397.9400086720375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4B16-8B4F-B8CB-8FB0C68535EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="988070319"/>
+        <c:axId val="1066103983"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="988070319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1066103983"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1066103983"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="988070319"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2371,6 +3006,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3384,6 +4059,522 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3477,11 +4668,47 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>388055</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>117122</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>797277</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>94544</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7C401F3-DA39-F951-4BB4-4CD9F2A7B80B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Djikstraout_1" connectionId="1" xr16:uid="{BA83A13A-C8EB-6542-8A48-6788935C5A3D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Djikstraout_1" connectionId="1" xr16:uid="{88E852B3-A2FD-974B-8D4E-22C6713E74C2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3783,8 +5010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3220C35-DA7E-8F42-A9AB-02907E785817}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="AC7" sqref="AC7"/>
+    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3844,16 +5071,16 @@
         <v>26</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2">
+        <v>22</v>
+      </c>
+      <c r="G2">
         <v>26</v>
       </c>
-      <c r="G2">
-        <v>23</v>
-      </c>
       <c r="H2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I2" s="1">
         <f>D2*LOG(C2)</f>
@@ -3874,16 +5101,16 @@
         <v>32</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I51" si="0">D3*LOG(C3)</f>
@@ -3910,10 +5137,10 @@
         <v>38</v>
       </c>
       <c r="G4">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
@@ -3940,10 +5167,10 @@
         <v>44</v>
       </c>
       <c r="G5">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H5">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
@@ -3970,10 +5197,10 @@
         <v>50</v>
       </c>
       <c r="G6">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H6">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
@@ -4000,10 +5227,10 @@
         <v>56</v>
       </c>
       <c r="G7">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H7">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
@@ -4030,10 +5257,10 @@
         <v>62</v>
       </c>
       <c r="G8">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
@@ -4060,10 +5287,10 @@
         <v>68</v>
       </c>
       <c r="G9">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="H9">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
@@ -4090,10 +5317,10 @@
         <v>74</v>
       </c>
       <c r="G10">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="H10">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
@@ -4120,10 +5347,10 @@
         <v>80</v>
       </c>
       <c r="G11">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="H11">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
@@ -4150,10 +5377,10 @@
         <v>104</v>
       </c>
       <c r="G12">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H12">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
@@ -4180,10 +5407,10 @@
         <v>128</v>
       </c>
       <c r="G13">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="H13">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
@@ -4210,10 +5437,10 @@
         <v>152</v>
       </c>
       <c r="G14">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="H14">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
@@ -4240,10 +5467,10 @@
         <v>176</v>
       </c>
       <c r="G15">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="H15">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="0"/>
@@ -4270,10 +5497,10 @@
         <v>200</v>
       </c>
       <c r="G16">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="H16">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="0"/>
@@ -4300,10 +5527,10 @@
         <v>224</v>
       </c>
       <c r="G17">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="H17">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="0"/>
@@ -4330,10 +5557,10 @@
         <v>248</v>
       </c>
       <c r="G18">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="H18">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="0"/>
@@ -4360,10 +5587,10 @@
         <v>272</v>
       </c>
       <c r="G19">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="H19">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="0"/>
@@ -4390,10 +5617,10 @@
         <v>296</v>
       </c>
       <c r="G20">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H20">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="0"/>
@@ -4420,10 +5647,10 @@
         <v>320</v>
       </c>
       <c r="G21">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="H21">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="0"/>
@@ -4450,10 +5677,10 @@
         <v>234</v>
       </c>
       <c r="G22">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="H22">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="0"/>
@@ -4480,10 +5707,10 @@
         <v>288</v>
       </c>
       <c r="G23">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="H23">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="0"/>
@@ -4510,10 +5737,10 @@
         <v>342</v>
       </c>
       <c r="G24">
-        <v>214</v>
+        <v>268</v>
       </c>
       <c r="H24">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="0"/>
@@ -4540,10 +5767,10 @@
         <v>396</v>
       </c>
       <c r="G25">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="H25">
-        <v>181</v>
+        <v>212</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="0"/>
@@ -4570,10 +5797,10 @@
         <v>450</v>
       </c>
       <c r="G26">
-        <v>249</v>
+        <v>217</v>
       </c>
       <c r="H26">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" si="0"/>
@@ -4600,10 +5827,10 @@
         <v>504</v>
       </c>
       <c r="G27">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="H27">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="0"/>
@@ -4630,10 +5857,10 @@
         <v>558</v>
       </c>
       <c r="G28">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="H28">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="I28" s="1">
         <f t="shared" si="0"/>
@@ -4660,10 +5887,10 @@
         <v>612</v>
       </c>
       <c r="G29">
-        <v>272</v>
+        <v>239</v>
       </c>
       <c r="H29">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="I29" s="1">
         <f t="shared" si="0"/>
@@ -4690,10 +5917,10 @@
         <v>666</v>
       </c>
       <c r="G30">
-        <v>262</v>
+        <v>232</v>
       </c>
       <c r="H30">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" si="0"/>
@@ -4720,10 +5947,10 @@
         <v>720</v>
       </c>
       <c r="G31">
-        <v>292</v>
+        <v>227</v>
       </c>
       <c r="H31">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="I31" s="1">
         <f t="shared" si="0"/>
@@ -4750,10 +5977,10 @@
         <v>416</v>
       </c>
       <c r="G32">
-        <v>281</v>
+        <v>381</v>
       </c>
       <c r="H32">
-        <v>222</v>
+        <v>287</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" si="0"/>
@@ -4780,7 +6007,7 @@
         <v>512</v>
       </c>
       <c r="G33">
-        <v>318</v>
+        <v>342</v>
       </c>
       <c r="H33">
         <v>243</v>
@@ -4810,10 +6037,10 @@
         <v>608</v>
       </c>
       <c r="G34">
-        <v>380</v>
+        <v>332</v>
       </c>
       <c r="H34">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="I34" s="1">
         <f t="shared" si="0"/>
@@ -4840,10 +6067,10 @@
         <v>704</v>
       </c>
       <c r="G35">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="H35">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I35" s="1">
         <f t="shared" si="0"/>
@@ -4870,10 +6097,10 @@
         <v>800</v>
       </c>
       <c r="G36">
-        <v>371</v>
+        <v>379</v>
       </c>
       <c r="H36">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="I36" s="1">
         <f t="shared" si="0"/>
@@ -4900,10 +6127,10 @@
         <v>896</v>
       </c>
       <c r="G37">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="H37">
-        <v>221</v>
+        <v>259</v>
       </c>
       <c r="I37" s="1">
         <f t="shared" si="0"/>
@@ -4930,10 +6157,10 @@
         <v>992</v>
       </c>
       <c r="G38">
-        <v>454</v>
+        <v>424</v>
       </c>
       <c r="H38">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="I38" s="1">
         <f t="shared" si="0"/>
@@ -4960,10 +6187,10 @@
         <v>1088</v>
       </c>
       <c r="G39">
-        <v>355</v>
+        <v>439</v>
       </c>
       <c r="H39">
-        <v>229</v>
+        <v>311</v>
       </c>
       <c r="I39" s="1">
         <f t="shared" si="0"/>
@@ -4990,10 +6217,10 @@
         <v>1184</v>
       </c>
       <c r="G40">
-        <v>421</v>
+        <v>385</v>
       </c>
       <c r="H40">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="I40" s="1">
         <f t="shared" si="0"/>
@@ -5020,10 +6247,10 @@
         <v>1280</v>
       </c>
       <c r="G41">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="H41">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="I41" s="1">
         <f t="shared" si="0"/>
@@ -5050,10 +6277,10 @@
         <v>650</v>
       </c>
       <c r="G42">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="H42">
-        <v>276</v>
+        <v>313</v>
       </c>
       <c r="I42" s="1">
         <f t="shared" si="0"/>
@@ -5080,10 +6307,10 @@
         <v>800</v>
       </c>
       <c r="G43">
-        <v>441</v>
+        <v>532</v>
       </c>
       <c r="H43">
-        <v>310</v>
+        <v>361</v>
       </c>
       <c r="I43" s="1">
         <f t="shared" si="0"/>
@@ -5110,10 +6337,10 @@
         <v>950</v>
       </c>
       <c r="G44">
-        <v>530</v>
+        <v>508</v>
       </c>
       <c r="H44">
-        <v>351</v>
+        <v>376</v>
       </c>
       <c r="I44" s="1">
         <f t="shared" si="0"/>
@@ -5140,10 +6367,10 @@
         <v>1100</v>
       </c>
       <c r="G45">
-        <v>561</v>
+        <v>575</v>
       </c>
       <c r="H45">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="I45" s="1">
         <f t="shared" si="0"/>
@@ -5170,10 +6397,10 @@
         <v>1250</v>
       </c>
       <c r="G46">
-        <v>542</v>
+        <v>575</v>
       </c>
       <c r="H46">
-        <v>337</v>
+        <v>378</v>
       </c>
       <c r="I46" s="1">
         <f t="shared" si="0"/>
@@ -5200,10 +6427,10 @@
         <v>1400</v>
       </c>
       <c r="G47">
-        <v>611</v>
+        <v>486</v>
       </c>
       <c r="H47">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" si="0"/>
@@ -5230,10 +6457,10 @@
         <v>1550</v>
       </c>
       <c r="G48">
-        <v>545</v>
+        <v>587</v>
       </c>
       <c r="H48">
-        <v>315</v>
+        <v>343</v>
       </c>
       <c r="I48" s="1">
         <f t="shared" si="0"/>
@@ -5260,10 +6487,10 @@
         <v>1700</v>
       </c>
       <c r="G49">
-        <v>600</v>
+        <v>575</v>
       </c>
       <c r="H49">
-        <v>350</v>
+        <v>287</v>
       </c>
       <c r="I49" s="1">
         <f t="shared" si="0"/>
@@ -5290,10 +6517,10 @@
         <v>1850</v>
       </c>
       <c r="G50">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="H50">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="I50" s="1">
         <f t="shared" si="0"/>
@@ -5320,10 +6547,10 @@
         <v>2000</v>
       </c>
       <c r="G51">
-        <v>580</v>
+        <v>608</v>
       </c>
       <c r="H51">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I51" s="1">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
added comments and updated make file and more excel graphs
</commit_message>
<xml_diff>
--- a/Graph Data Visualised.xlsx
+++ b/Graph Data Visualised.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahgonsenhauser/Dropbox/UCT/CSC2001F/Assignment5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E5460C-6E00-504B-91EB-E2960E93B896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7577BE-2B5F-C844-94AE-98FE3C76B84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{D305D5BE-1447-6B45-9963-199F3DD44BDD}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{38526DA4-F952-E341-9F1B-A50F21DB8BBC}" name="Djikstraout" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/noahgonsenhauser/Dropbox/UCT/CSC2001F/Assignment5/Djikstraout.txt" decimal="," thousands=" " tab="0" space="1" consecutive="1">
+    <textPr sourceFile="/Users/noahgonsenhauser/Dropbox/UCT/CSC2001F/Assignment5/Djikstraout.txt" decimal="," thousands=" " tab="0" space="1" consecutive="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>graph</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>O Complexity (|E|log|V|)</t>
+  </si>
+  <si>
+    <t>E + V Operations</t>
   </si>
 </sst>
 </file>
@@ -2306,6 +2309,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>PQ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Operations vs O Complexity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2926,6 +2959,1975 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PQOperations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>342</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>391</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>508</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>587</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>549</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>608</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-41EE-9941-B5CB-BAAD66A9B775}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="821163984"/>
+        <c:axId val="821166688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="821163984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="821166688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="821166688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="821163984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PQ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Operations vs</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> Complexity (|E|log|V|)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.30068744531933506"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>O Complexity (|E|log|V|)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>342</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>391</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>508</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>587</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>549</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>608</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>135.30711954905405</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>166.5318394449896</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>197.75655934092515</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>228.9812792368607</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>260.20599913279625</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>291.4307190287318</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>322.65543892466735</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>353.8801588206029</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>385.10487871653845</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>416.329598612474</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>345.64637360440099</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>425.41092135926277</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>505.17546911412455</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>584.94001686898628</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>664.70456462384811</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>744.46911237870984</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>824.23366013357156</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>903.9982078884334</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>983.76275564329512</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1063.5273033981568</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>666.45695639243229</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>820.25471555991669</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>974.05247472740109</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1127.8502338948854</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1281.6479930623698</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1435.4457522298542</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1589.2435113973386</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1743.041270564823</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1896.8390297323074</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2050.6367888997916</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1104.3305028184122</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1359.176003468815</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1614.0215041192178</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1868.8670047696205</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2123.7125054200233</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2378.558006070426</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2633.4035067208292</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2888.249007371232</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3143.0945080216347</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3397.9400086720375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C9D2-234C-B916-14ADD5699008}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="552749840"/>
+        <c:axId val="552752544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="552749840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>PQ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Operations</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="552752544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="552752544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>O</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Complexity</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="552749840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>E + V Operations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$51</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>135.30711954905405</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>166.5318394449896</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>197.75655934092515</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>228.9812792368607</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>260.20599913279625</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>291.4307190287318</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>322.65543892466735</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>353.8801588206029</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>385.10487871653845</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>416.329598612474</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>345.64637360440099</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>425.41092135926277</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>505.17546911412455</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>584.94001686898628</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>664.70456462384811</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>744.46911237870984</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>824.23366013357156</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>903.9982078884334</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>983.76275564329512</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1063.5273033981568</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>666.45695639243229</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>820.25471555991669</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>974.05247472740109</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1127.8502338948854</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1281.6479930623698</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1435.4457522298542</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1589.2435113973386</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1743.041270564823</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1896.8390297323074</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2050.6367888997916</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1104.3305028184122</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1359.176003468815</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1614.0215041192178</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1868.8670047696205</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2123.7125054200233</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2378.558006070426</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2633.4035067208292</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2888.249007371232</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3143.0945080216347</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3397.9400086720375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>372</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>534</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>588</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>552</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>648</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>744</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>936</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1032</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1128</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1224</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-356E-EE41-AA95-A40F65F10E35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="579151936"/>
+        <c:axId val="579154208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="579151936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="579154208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="579154208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="579151936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3046,6 +5048,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4594,20 +6716,1568 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>157316</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>512916</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>138470</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>265373</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>50799</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>577144</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>141111</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4634,16 +8304,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>130791</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>78475</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>655725</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>188542</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>284328</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>151642</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>541867</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>135467</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4670,16 +8340,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>388055</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>117122</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>732959</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>40031</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>797277</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>94544</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>67733</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>186267</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4699,6 +8369,114 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>382783</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>160866</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54FE0805-ABEB-F98F-C716-134F05E809F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>131234</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>194734</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FF1FEA1-6D78-F54E-78ED-1244F331CF01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>299837</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>178384</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>723169</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>75617</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99A140DF-29E1-C06D-F7AB-B68571A8A05C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5008,10 +8786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3220C35-DA7E-8F42-A9AB-02907E785817}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5025,10 +8803,11 @@
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="15" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1"/>
+    <col min="11" max="15" width="3.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5056,8 +8835,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5086,8 +8868,12 @@
         <f>D2*LOG(C2)</f>
         <v>26</v>
       </c>
+      <c r="J2">
+        <f>E2+F2</f>
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5116,8 +8902,12 @@
         <f t="shared" ref="I3:I51" si="0">D3*LOG(C3)</f>
         <v>32</v>
       </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J51" si="1">E3+F3</f>
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5146,8 +8936,12 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5176,8 +8970,12 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -5206,8 +9004,12 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -5236,8 +9038,12 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -5266,8 +9072,12 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -5296,8 +9106,12 @@
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -5326,8 +9140,12 @@
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5356,8 +9174,12 @@
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -5386,8 +9208,12 @@
         <f t="shared" si="0"/>
         <v>135.30711954905405</v>
       </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -5416,8 +9242,12 @@
         <f t="shared" si="0"/>
         <v>166.5318394449896</v>
       </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>148</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -5446,8 +9276,12 @@
         <f t="shared" si="0"/>
         <v>197.75655934092515</v>
       </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>172</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -5476,8 +9310,12 @@
         <f t="shared" si="0"/>
         <v>228.9812792368607</v>
       </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -5506,8 +9344,12 @@
         <f t="shared" si="0"/>
         <v>260.20599913279625</v>
       </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -5536,8 +9378,12 @@
         <f t="shared" si="0"/>
         <v>291.4307190287318</v>
       </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>244</v>
+      </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -5566,8 +9412,12 @@
         <f t="shared" si="0"/>
         <v>322.65543892466735</v>
       </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>268</v>
+      </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -5596,8 +9446,12 @@
         <f t="shared" si="0"/>
         <v>353.8801588206029</v>
       </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>292</v>
+      </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -5626,8 +9480,12 @@
         <f t="shared" si="0"/>
         <v>385.10487871653845</v>
       </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>316</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -5656,8 +9514,12 @@
         <f t="shared" si="0"/>
         <v>416.329598612474</v>
       </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>340</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -5686,8 +9548,12 @@
         <f t="shared" si="0"/>
         <v>345.64637360440099</v>
       </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>264</v>
+      </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -5716,8 +9582,12 @@
         <f t="shared" si="0"/>
         <v>425.41092135926277</v>
       </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>318</v>
+      </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -5746,8 +9616,12 @@
         <f t="shared" si="0"/>
         <v>505.17546911412455</v>
       </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>372</v>
+      </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5776,8 +9650,12 @@
         <f t="shared" si="0"/>
         <v>584.94001686898628</v>
       </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>426</v>
+      </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5806,8 +9684,12 @@
         <f t="shared" si="0"/>
         <v>664.70456462384811</v>
       </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5836,8 +9718,12 @@
         <f t="shared" si="0"/>
         <v>744.46911237870984</v>
       </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>534</v>
+      </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5866,8 +9752,12 @@
         <f t="shared" si="0"/>
         <v>824.23366013357156</v>
       </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>588</v>
+      </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5896,8 +9786,12 @@
         <f t="shared" si="0"/>
         <v>903.9982078884334</v>
       </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>642</v>
+      </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5926,8 +9820,12 @@
         <f t="shared" si="0"/>
         <v>983.76275564329512</v>
       </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>696</v>
+      </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5956,8 +9854,12 @@
         <f t="shared" si="0"/>
         <v>1063.5273033981568</v>
       </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5986,8 +9888,12 @@
         <f t="shared" si="0"/>
         <v>666.45695639243229</v>
       </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>456</v>
+      </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -6016,8 +9922,12 @@
         <f t="shared" si="0"/>
         <v>820.25471555991669</v>
       </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>552</v>
+      </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -6046,8 +9956,12 @@
         <f t="shared" si="0"/>
         <v>974.05247472740109</v>
       </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>648</v>
+      </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -6076,8 +9990,12 @@
         <f t="shared" si="0"/>
         <v>1127.8502338948854</v>
       </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>744</v>
+      </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -6106,8 +10024,12 @@
         <f t="shared" si="0"/>
         <v>1281.6479930623698</v>
       </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>840</v>
+      </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -6136,8 +10058,12 @@
         <f t="shared" si="0"/>
         <v>1435.4457522298542</v>
       </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>936</v>
+      </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -6166,8 +10092,12 @@
         <f t="shared" si="0"/>
         <v>1589.2435113973386</v>
       </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>1032</v>
+      </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -6196,8 +10126,12 @@
         <f t="shared" si="0"/>
         <v>1743.041270564823</v>
       </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>1128</v>
+      </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -6226,8 +10160,12 @@
         <f t="shared" si="0"/>
         <v>1896.8390297323074</v>
       </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>1224</v>
+      </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -6256,8 +10194,12 @@
         <f t="shared" si="0"/>
         <v>2050.6367888997916</v>
       </c>
+      <c r="J41">
+        <f t="shared" si="1"/>
+        <v>1320</v>
+      </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -6286,8 +10228,12 @@
         <f t="shared" si="0"/>
         <v>1104.3305028184122</v>
       </c>
+      <c r="J42">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -6316,8 +10262,12 @@
         <f t="shared" si="0"/>
         <v>1359.176003468815</v>
       </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>850</v>
+      </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -6346,8 +10296,12 @@
         <f t="shared" si="0"/>
         <v>1614.0215041192178</v>
       </c>
+      <c r="J44">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -6376,8 +10330,12 @@
         <f t="shared" si="0"/>
         <v>1868.8670047696205</v>
       </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>1150</v>
+      </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -6406,8 +10364,12 @@
         <f t="shared" si="0"/>
         <v>2123.7125054200233</v>
       </c>
+      <c r="J46">
+        <f t="shared" si="1"/>
+        <v>1300</v>
+      </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -6436,8 +10398,12 @@
         <f t="shared" si="0"/>
         <v>2378.558006070426</v>
       </c>
+      <c r="J47">
+        <f t="shared" si="1"/>
+        <v>1450</v>
+      </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -6466,8 +10432,12 @@
         <f t="shared" si="0"/>
         <v>2633.4035067208292</v>
       </c>
+      <c r="J48">
+        <f t="shared" si="1"/>
+        <v>1600</v>
+      </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -6496,8 +10466,12 @@
         <f t="shared" si="0"/>
         <v>2888.249007371232</v>
       </c>
+      <c r="J49">
+        <f t="shared" si="1"/>
+        <v>1750</v>
+      </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -6526,8 +10500,12 @@
         <f t="shared" si="0"/>
         <v>3143.0945080216347</v>
       </c>
+      <c r="J50">
+        <f t="shared" si="1"/>
+        <v>1900</v>
+      </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -6555,6 +10533,10 @@
       <c r="I51" s="1">
         <f t="shared" si="0"/>
         <v>3397.9400086720375</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="1"/>
+        <v>2050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>